<commit_message>
changed names Id10008_check to Id1008_check
</commit_message>
<xml_diff>
--- a/WHOVA2016_v1_5_1_XLS_form_for_ODK.xlsx
+++ b/WHOVA2016_v1_5_1_XLS_form_for_ODK.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT_FOLDER\WHO_VA_2016\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="465" windowWidth="11175" windowHeight="7560" activeTab="2"/>
+    <workbookView xWindow="4188" yWindow="468" windowWidth="11172" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -6420,12 +6425,6 @@
     <t>(selected(${Id10235}, 'DK') or selected(${Id10235}, 'Ref')) and count-selected(${Id10235})&gt;1</t>
   </si>
   <si>
-    <t>Id10008_check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Id10008_check) It is not possible to select that the respondent is the child of the deceased and enter that the deceased is a neonate or child. Please go back and correct the selection. </t>
-  </si>
-  <si>
     <t>(selected(${Id10114}, 'no') or ${Id10114} = 'NaN' or string-length(${Id10114}) = 0) and selected(${isNeonatal}, '1') and (selected(${Id10098}, 'yes') or ${Id10098} = 'NaN' or string-length(${Id10098}) = 0)   and not(selected(${Id10099}, 'yes'))</t>
   </si>
   <si>
@@ -6436,12 +6435,18 @@
   </si>
   <si>
     <t>2016 WHO Verbal Autopsy Form 1.5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Id1008_check) It is not possible to select that the respondent is the child of the deceased and enter that the deceased is a neonate or child. Please go back and correct the selection. </t>
+  </si>
+  <si>
+    <t>Id1008_check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="38">
     <font>
       <sz val="11"/>
@@ -7317,24 +7322,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1020"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.6" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="28" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="76.42578125" style="39" customWidth="1"/>
-    <col min="4" max="4" width="79.85546875" style="39" customWidth="1"/>
-    <col min="5" max="5" width="147.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="76.44140625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="79.88671875" style="39" customWidth="1"/>
+    <col min="5" max="5" width="147.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6" customWidth="1"/>
     <col min="9" max="10" width="82" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="45" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="6"/>
+    <col min="14" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.6" customHeight="1">
@@ -7386,7 +7391,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="90" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="D2" s="38"/>
     </row>
@@ -8250,10 +8255,10 @@
         <v>619</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>2076</v>
+        <v>2081</v>
       </c>
       <c r="C56" s="38" t="s">
-        <v>2077</v>
+        <v>2080</v>
       </c>
       <c r="D56" s="38"/>
       <c r="E56" s="1" t="s">
@@ -9422,7 +9427,7 @@
         <v>1315</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>14</v>
@@ -19642,13 +19647,13 @@
       <selection activeCell="A171" sqref="A171:A172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="45.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="45.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="45.140625" style="2"/>
+    <col min="1" max="1" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="45.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -23649,16 +23654,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="49.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.44140625" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -23680,13 +23685,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="B2" s="27">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="D2" t="s">
         <v>514</v>

</xml_diff>